<commit_message>
Changes made to the frontend to auto push bulk WA messages
</commit_message>
<xml_diff>
--- a/EnquiryList.xlsx
+++ b/EnquiryList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\auto-whatsapp-message\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CE4D7F-AC4A-4139-AC49-67DA109EC9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A9764C-689A-4838-BF35-46E04EEEB2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EnquiryList" sheetId="3" r:id="rId1"/>
@@ -1240,13 +1240,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE1C842-76FE-4BB7-9F64-45E6CC68223D}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2956,7 +2957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AAC5C8-C54E-47BC-BFA2-70939FE2F545}">
   <dimension ref="C1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>

</xml_diff>